<commit_message>
Ticket creation page added. Login information extraction remaining
</commit_message>
<xml_diff>
--- a/Data Model.xlsx
+++ b/Data Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santosh Kannan\Desktop\UF\ResumeProjects\BugTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1262796-3719-463F-A117-D690631AE35B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE7E7FC-8342-49AA-93B3-DB117DE0726B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9AE1D6F-56C5-4333-8C24-04A3E057554A}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>t_desc</t>
   </si>
   <si>
-    <t>t_submitter</t>
-  </si>
-  <si>
     <t>p_id</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>t_type</t>
+  </si>
+  <si>
+    <t>submitter_id</t>
   </si>
 </sst>
 </file>
@@ -200,10 +200,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -524,7 +524,7 @@
   <dimension ref="C4:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,291 +541,291 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="G4" s="1" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="O4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+    </row>
+    <row r="5" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="K4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="O4" s="1" t="s">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="O7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="3"/>
+      <c r="S7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="O8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="S8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="S4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-    </row>
-    <row r="5" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="K9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="O9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="S9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="O10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="S10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="K6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="K7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="O7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="3"/>
-      <c r="S7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="K8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="O8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="S8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-    </row>
-    <row r="9" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="K9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="O9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="S9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-    </row>
-    <row r="10" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="K10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="O10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="S10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-    </row>
-    <row r="11" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="S4:U4"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="S4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added models for employee and developer
</commit_message>
<xml_diff>
--- a/Data Model.xlsx
+++ b/Data Model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santosh Kannan\Desktop\UF\ResumeProjects\BugTracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UF\ResumeProjects\BugTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE7E7FC-8342-49AA-93B3-DB117DE0726B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84893B46-8800-4AB4-BB83-61C12A3C0A15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9AE1D6F-56C5-4333-8C24-04A3E057554A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Ticket</t>
   </si>
@@ -105,9 +105,6 @@
     <t>assign_date</t>
   </si>
   <si>
-    <t>Candidate key</t>
-  </si>
-  <si>
     <t>p_start_date</t>
   </si>
   <si>
@@ -148,6 +145,12 @@
   </si>
   <si>
     <t>submitter_id</t>
+  </si>
+  <si>
+    <t>update_date</t>
+  </si>
+  <si>
+    <t>map_id</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -194,11 +197,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -207,6 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +539,7 @@
   <dimension ref="C4:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="Q7" sqref="Q7:Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,7 +634,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
@@ -637,11 +652,11 @@
         <v>5</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="P6" s="1"/>
-      <c r="Q6" s="3" t="s">
-        <v>23</v>
+      <c r="Q6" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>20</v>
@@ -656,7 +671,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -670,12 +685,12 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="O7" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="3"/>
       <c r="S7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -685,7 +700,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1"/>
       <c r="K8" s="1" t="s">
@@ -694,12 +709,12 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="O8" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="3"/>
       <c r="S8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -709,45 +724,45 @@
         <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="S9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
     <row r="10" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="S10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -757,13 +772,18 @@
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="O11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
       <c r="S11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -773,25 +793,28 @@
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1"/>
+      <c r="S12" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -800,32 +823,32 @@
         <v>13</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="Q7:Q8"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="Q6:Q7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added ticket details page
</commit_message>
<xml_diff>
--- a/Data Model.xlsx
+++ b/Data Model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UF\ResumeProjects\BugTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84893B46-8800-4AB4-BB83-61C12A3C0A15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D099659-544B-4433-8430-A7A770CB5E4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9AE1D6F-56C5-4333-8C24-04A3E057554A}"/>
   </bookViews>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
-  <si>
-    <t>Ticket</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>Column name</t>
   </si>
@@ -78,9 +72,6 @@
     <t>t_create_date</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -151,6 +142,24 @@
   </si>
   <si>
     <t>map_id</t>
+  </si>
+  <si>
+    <t>ticket_details</t>
+  </si>
+  <si>
+    <t>ticket</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>t_update_date</t>
+  </si>
+  <si>
+    <t>t_detail_id</t>
   </si>
 </sst>
 </file>
@@ -174,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -197,17 +206,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -216,12 +214,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F29C63-09CB-4A70-8D20-E9F2F4108E82}">
-  <dimension ref="C4:U20"/>
+  <dimension ref="C4:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7:Q8"/>
+      <selection activeCell="S4" sqref="S4:U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,296 +548,355 @@
     <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.21875" customWidth="1"/>
+    <col min="17" max="17" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:21" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="K4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="O4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="S4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="S4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
     </row>
     <row r="5" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="K5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="O5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="O7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="3"/>
+      <c r="Q7" s="2"/>
       <c r="S7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
     <row r="8" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1"/>
       <c r="K8" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="O8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P8" s="1"/>
-      <c r="Q8" s="3"/>
+      <c r="Q8" s="2"/>
       <c r="S8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
     <row r="9" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="S9" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
     <row r="10" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="S10" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
     <row r="11" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="S11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
     <row r="12" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1"/>
       <c r="S12" s="4" t="s">
-        <v>37</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
     </row>
     <row r="13" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="1"/>
       <c r="G20" t="s">
-        <v>31</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>